<commit_message>
direct commit. added new customer 1010
</commit_message>
<xml_diff>
--- a/test3.xlsx
+++ b/test3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47779A7D-5B2C-4F39-BFC1-518030ABE3A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC42EB2-776A-4662-B3EC-77BBD2BC38BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Cust Id </t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>PQR</t>
+  </si>
+  <si>
+    <t>STU</t>
+  </si>
+  <si>
+    <t>VWX</t>
   </si>
 </sst>
 </file>
@@ -364,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,6 +422,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1010</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
first change made in branch1
</commit_message>
<xml_diff>
--- a/test3.xlsx
+++ b/test3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC42EB2-776A-4662-B3EC-77BBD2BC38BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177B88DB-599B-48C9-A54C-0FE2F6D1D6FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Cust Id </t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t>VWX</t>
+  </si>
+  <si>
+    <t>cccc</t>
+  </si>
+  <si>
+    <t>vvvv</t>
+  </si>
+  <si>
+    <t>line added from myproject1-branch1</t>
   </si>
 </sst>
 </file>
@@ -370,15 +379,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,7 +398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>123</v>
       </c>
@@ -400,7 +409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>456</v>
       </c>
@@ -411,7 +420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>789</v>
       </c>
@@ -422,7 +431,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1010</v>
       </c>
@@ -431,6 +440,20 @@
       </c>
       <c r="C5" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2020</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
one more change in branch
</commit_message>
<xml_diff>
--- a/test3.xlsx
+++ b/test3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177B88DB-599B-48C9-A54C-0FE2F6D1D6FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E87D08-1A9B-4122-BA51-954167D9B5E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Cust Id </t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t>line added from myproject1-branch1</t>
+  </si>
+  <si>
+    <t>dddd</t>
+  </si>
+  <si>
+    <t>zzzz</t>
+  </si>
+  <si>
+    <t>2nd line added</t>
   </si>
 </sst>
 </file>
@@ -379,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,6 +465,20 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4040</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>